<commit_message>
Nawiazanie polaczenia w serwerze smiga
</commit_message>
<xml_diff>
--- a/docs/API.xlsx
+++ b/docs/API.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="106">
   <si>
     <t xml:space="preserve">Projekt TIN</t>
   </si>
@@ -52,9 +52,6 @@
     <t xml:space="preserve">CL_CONNECTION_REQ </t>
   </si>
   <si>
-    <t xml:space="preserve">Request</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Server: </t>
   </si>
   <si>
@@ -74,9 +71,6 @@
   </si>
   <si>
     <t xml:space="preserve">SRV_CHALLENGE_ACC </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Return</t>
   </si>
   <si>
     <t xml:space="preserve">CL_SSID_REQ </t>
@@ -489,18 +483,18 @@
   </sheetPr>
   <dimension ref="A1:F116"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.1052631578947"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.2105263157895"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="7.71255060728745"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="24.6356275303644"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="28.8137651821862"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="33.1012145748988"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="24.8502024291498"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="29.0283400809717"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="33.4210526315789"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="25.8137651821862"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -584,7 +578,7 @@
       <c r="E8" s="4"/>
       <c r="F8" s="0"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2"/>
       <c r="B9" s="1" t="n">
         <v>1</v>
@@ -595,9 +589,7 @@
       <c r="D9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="E9" s="4"/>
       <c r="F9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -606,13 +598,13 @@
         <v>2</v>
       </c>
       <c r="C10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="E10" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>13</v>
       </c>
       <c r="F10" s="0"/>
     </row>
@@ -625,29 +617,27 @@
         <v>8</v>
       </c>
       <c r="D11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="F11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2"/>
       <c r="B12" s="1" t="n">
         <v>4</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>18</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="E12" s="4"/>
       <c r="F12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -659,10 +649,10 @@
         <v>8</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F13" s="0"/>
     </row>
@@ -672,30 +662,30 @@
         <v>6</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2"/>
       <c r="B15" s="0"/>
       <c r="C15" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -707,10 +697,10 @@
         <v>8</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F16" s="0"/>
     </row>
@@ -720,15 +710,15 @@
         <v>8</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="0"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2"/>
       <c r="B18" s="0"/>
       <c r="C18" s="4"/>
@@ -746,7 +736,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B20" s="0"/>
       <c r="C20" s="4"/>
@@ -760,12 +750,12 @@
         <v>1</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -774,12 +764,12 @@
         <v>2</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
       <c r="F22" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -800,7 +790,7 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B25" s="0"/>
       <c r="C25" s="4"/>
@@ -809,44 +799,47 @@
       <c r="F25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0"/>
       <c r="B26" s="5" t="n">
         <v>1</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0"/>
       <c r="B27" s="5" t="n">
         <v>2</v>
       </c>
       <c r="C27" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E27" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="F27" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="E27" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F27" s="0" t="s">
-        <v>40</v>
-      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0"/>
       <c r="B28" s="5" t="n">
         <v>3</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E28" s="4"/>
       <c r="F28" s="0"/>
@@ -869,14 +862,14 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B31" s="0"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
       <c r="F31" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -885,13 +878,13 @@
         <v>1</v>
       </c>
       <c r="C32" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E32" s="4" t="s">
         <v>44</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>46</v>
       </c>
       <c r="F32" s="0"/>
     </row>
@@ -901,10 +894,10 @@
         <v>2</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E33" s="4"/>
       <c r="F33" s="0"/>
@@ -915,13 +908,13 @@
         <v>3</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F34" s="0"/>
     </row>
@@ -931,13 +924,13 @@
         <v>4</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F35" s="0"/>
     </row>
@@ -947,13 +940,13 @@
         <v>5</v>
       </c>
       <c r="C36" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E36" s="4" t="s">
         <v>53</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>55</v>
       </c>
       <c r="F36" s="0"/>
     </row>
@@ -963,10 +956,10 @@
         <v>6</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E37" s="4" t="n">
         <v>1</v>
@@ -979,13 +972,13 @@
         <v>7</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F38" s="0"/>
     </row>
@@ -995,10 +988,10 @@
         <v>8</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E39" s="4" t="n">
         <v>2</v>
@@ -1016,61 +1009,61 @@
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2"/>
       <c r="B41" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F41" s="0"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2"/>
       <c r="B42" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F42" s="0"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2"/>
       <c r="B43" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F43" s="0"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2"/>
       <c r="B44" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E44" s="4"/>
       <c r="F44" s="0"/>
@@ -1093,7 +1086,7 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B47" s="0"/>
       <c r="C47" s="4"/>
@@ -1107,16 +1100,16 @@
         <v>1</v>
       </c>
       <c r="C48" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E48" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D48" s="4" t="s">
+      <c r="F48" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="E48" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1125,16 +1118,16 @@
         <v>2</v>
       </c>
       <c r="C49" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E49" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D49" s="4" t="s">
+      <c r="F49" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="E49" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1143,13 +1136,13 @@
         <v>3</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1158,10 +1151,10 @@
         <v>4</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E51" s="4"/>
     </row>
@@ -1171,13 +1164,13 @@
         <v>5</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1186,10 +1179,10 @@
         <v>6</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E53" s="4"/>
     </row>
@@ -1199,13 +1192,13 @@
         <v>7</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1214,10 +1207,10 @@
         <v>8</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E55" s="4" t="n">
         <v>1</v>
@@ -1229,13 +1222,13 @@
         <v>9</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1244,10 +1237,10 @@
         <v>10</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E57" s="4" t="n">
         <v>2</v>
@@ -1263,58 +1256,58 @@
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="2"/>
       <c r="B59" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="2"/>
       <c r="B60" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="2"/>
       <c r="B61" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="2"/>
       <c r="B62" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E62" s="4"/>
     </row>
@@ -1344,7 +1337,7 @@
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B69" s="0"/>
     </row>
@@ -1353,7 +1346,7 @@
         <v>1</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1361,7 +1354,7 @@
         <v>2</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1369,7 +1362,7 @@
         <v>3</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1377,7 +1370,7 @@
         <v>4</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1385,7 +1378,7 @@
         <v>5</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1393,7 +1386,7 @@
         <v>6</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1401,7 +1394,7 @@
         <v>7</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1409,7 +1402,7 @@
         <v>8</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1417,7 +1410,7 @@
         <v>9</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1431,7 +1424,7 @@
         <v>11</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1439,7 +1432,7 @@
         <v>12</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1495,7 +1488,7 @@
         <v>21</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1503,7 +1496,7 @@
         <v>22</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1511,7 +1504,7 @@
         <v>23</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1519,7 +1512,7 @@
         <v>24</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1527,7 +1520,7 @@
         <v>25</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1535,7 +1528,7 @@
         <v>26</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1543,7 +1536,7 @@
         <v>27</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1551,7 +1544,7 @@
         <v>28</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1559,7 +1552,7 @@
         <v>29</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1573,7 +1566,7 @@
         <v>31</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1581,7 +1574,7 @@
         <v>32</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1589,7 +1582,7 @@
         <v>33</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1597,7 +1590,7 @@
         <v>34</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1605,7 +1598,7 @@
         <v>35</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1613,7 +1606,7 @@
         <v>36</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1621,7 +1614,7 @@
         <v>37</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1647,7 +1640,7 @@
         <v>41</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1655,7 +1648,7 @@
         <v>42</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1663,22 +1656,29 @@
         <v>43</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="1" t="n">
         <v>44</v>
       </c>
-    </row>
-    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="B113" s="0"/>
+    </row>
+    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="0"/>
+      <c r="B114" s="0"/>
+    </row>
+    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="0"/>
+      <c r="B115" s="0"/>
+    </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="1" t="n">
         <v>90</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>